<commit_message>
Optimize Streamlit startup and lazy-load models
</commit_message>
<xml_diff>
--- a/forecast_summary.xlsx
+++ b/forecast_summary.xlsx
@@ -148,7 +148,7 @@
     <t>4th</t>
   </si>
   <si>
-    <t>Random Forest ranked 4th based on RMSE of 180800.49. It performs well for short-term, interpretable.</t>
+    <t>Random Forest ranked 4th based on RMSE of 165164.31. It performs well for short-term, interpretable.</t>
   </si>
   <si>
     <t>Exponential Smoothing</t>
@@ -595,7 +595,7 @@
         <v>40</v>
       </c>
       <c r="C5">
-        <v>180800.4885686614</v>
+        <v>165164.3121258343</v>
       </c>
       <c r="D5" t="s">
         <v>41</v>
@@ -1336,7 +1336,7 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>19827998.46055355</v>
+        <v>20009580.75716664</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1344,7 +1344,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>20323832.13575398</v>
+        <v>20505414.43236707</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1352,7 +1352,7 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>20540593.99132929</v>
+        <v>20722176.28794238</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1360,7 +1360,7 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>20057768.56594399</v>
+        <v>20239350.86255708</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1368,7 +1368,7 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>20411940.9652482</v>
+        <v>20593523.26186129</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1376,7 +1376,7 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>20692599.82232508</v>
+        <v>20874182.11893817</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1384,7 +1384,7 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>21031408.39085545</v>
+        <v>21212990.68746854</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1392,7 +1392,7 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <v>21866669.73352069</v>
+        <v>22048252.03013377</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1400,7 +1400,7 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <v>22288410.28174167</v>
+        <v>22469992.57835477</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1408,7 +1408,7 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>23198796.12933894</v>
+        <v>23380378.42595203</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1416,7 +1416,7 @@
         <v>19</v>
       </c>
       <c r="B12">
-        <v>23835437.05943865</v>
+        <v>24014981.72558681</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1432,7 +1432,7 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <v>19827998.46055355</v>
+        <v>20009580.75716664</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1440,7 +1440,7 @@
         <v>22</v>
       </c>
       <c r="B15">
-        <v>20323832.13575398</v>
+        <v>20505414.43236707</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1448,7 +1448,7 @@
         <v>23</v>
       </c>
       <c r="B16">
-        <v>20540593.99132929</v>
+        <v>20722176.28794238</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1456,7 +1456,7 @@
         <v>24</v>
       </c>
       <c r="B17">
-        <v>20057768.56594399</v>
+        <v>20239350.86255708</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1464,7 +1464,7 @@
         <v>25</v>
       </c>
       <c r="B18">
-        <v>20411940.9652482</v>
+        <v>20593523.26186129</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1472,7 +1472,7 @@
         <v>26</v>
       </c>
       <c r="B19">
-        <v>20692599.82232508</v>
+        <v>20874182.11893817</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1480,7 +1480,7 @@
         <v>27</v>
       </c>
       <c r="B20">
-        <v>21031408.39085545</v>
+        <v>21212990.68746854</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1488,7 +1488,7 @@
         <v>28</v>
       </c>
       <c r="B21">
-        <v>21866669.73352069</v>
+        <v>22048252.03013377</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1496,7 +1496,7 @@
         <v>29</v>
       </c>
       <c r="B22">
-        <v>22288410.28174167</v>
+        <v>22469992.57835477</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1504,7 +1504,7 @@
         <v>30</v>
       </c>
       <c r="B23">
-        <v>23198796.12933894</v>
+        <v>23380378.42595203</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1512,7 +1512,7 @@
         <v>31</v>
       </c>
       <c r="B24">
-        <v>23835437.05943865</v>
+        <v>24014981.72558681</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1549,7 +1549,7 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>20474000</v>
+        <v>20596000</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>20548000</v>
+        <v>20664000</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1565,7 +1565,7 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>20672000</v>
+        <v>20803000</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1573,7 +1573,7 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>20595000</v>
+        <v>20719000</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1581,7 +1581,7 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>20628000</v>
+        <v>20772000</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1589,7 +1589,7 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>20874000</v>
+        <v>21148000</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1597,7 +1597,7 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>21457000</v>
+        <v>21650000</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1605,7 +1605,7 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <v>21927000</v>
+        <v>21959000</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1613,7 +1613,7 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <v>22190000</v>
+        <v>22228000</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1621,7 +1621,7 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>22921000</v>
+        <v>22889000</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1629,7 +1629,7 @@
         <v>19</v>
       </c>
       <c r="B12">
-        <v>23469000</v>
+        <v>23496000</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1637,7 +1637,7 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <v>24010000</v>
+        <v>24100000</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1645,7 +1645,7 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <v>20474000</v>
+        <v>20596000</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1653,7 +1653,7 @@
         <v>22</v>
       </c>
       <c r="B15">
-        <v>20548000</v>
+        <v>20664000</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1661,7 +1661,7 @@
         <v>23</v>
       </c>
       <c r="B16">
-        <v>20672000</v>
+        <v>20803000</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1669,7 +1669,7 @@
         <v>24</v>
       </c>
       <c r="B17">
-        <v>20595000</v>
+        <v>20719000</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1677,7 +1677,7 @@
         <v>25</v>
       </c>
       <c r="B18">
-        <v>20628000</v>
+        <v>20772000</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1685,7 +1685,7 @@
         <v>26</v>
       </c>
       <c r="B19">
-        <v>20874000</v>
+        <v>21148000</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1693,7 +1693,7 @@
         <v>27</v>
       </c>
       <c r="B20">
-        <v>21457000</v>
+        <v>21650000</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1701,7 +1701,7 @@
         <v>28</v>
       </c>
       <c r="B21">
-        <v>21927000</v>
+        <v>21959000</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1709,7 +1709,7 @@
         <v>29</v>
       </c>
       <c r="B22">
-        <v>22190000</v>
+        <v>22228000</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1717,7 +1717,7 @@
         <v>30</v>
       </c>
       <c r="B23">
-        <v>22921000</v>
+        <v>22889000</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1725,7 +1725,7 @@
         <v>31</v>
       </c>
       <c r="B24">
-        <v>23469000</v>
+        <v>23496000</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1733,7 +1733,7 @@
         <v>32</v>
       </c>
       <c r="B25">
-        <v>24010000</v>
+        <v>24100000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>